<commit_message>
added mse to saved_results.xlsx
</commit_message>
<xml_diff>
--- a/data_loader/configs/saved_results.xlsx
+++ b/data_loader/configs/saved_results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -402,6 +402,11 @@
           <t>F_1_score</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>mse</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -434,6 +439,9 @@
       <c r="H2" t="n">
         <v>0.7400987056466867</v>
       </c>
+      <c r="I2" t="n">
+        <v>0.8011432342852155</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -461,10 +469,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.5675390625</v>
+        <v>0.5937239583333334</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6947237902965893</v>
+        <v>0.7365552616033121</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.7594823141892751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>